<commit_message>
desloc para total planilha resumo vendas
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/6.Funcoes_Mercado/14.Exercicios_finais/1.Trancamento_Parcial.xlsx
+++ b/2.Excel/hands-on/6.Funcoes_Mercado/14.Exercicios_finais/1.Trancamento_Parcial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\6.Funcoes_Mercado\14.Exercicios_finais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC6B058-18D2-4A88-81FF-B62FE83A71A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCFCEB1-AA36-4C1C-9D2D-05C9FECB50B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12240" yWindow="132" windowWidth="10800" windowHeight="12792" tabRatio="862" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12240" yWindow="132" windowWidth="10800" windowHeight="12792" tabRatio="862" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -18217,8 +18217,8 @@
   </sheetPr>
   <dimension ref="B1:I20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -18453,7 +18453,10 @@
       <c r="G12" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="H12" s="94"/>
+      <c r="H12" s="94">
+        <f ca="1">OFFSET(B8,MATCH(H10,B9:B20,0),MATCH(H9,C8:E8,0))</f>
+        <v>512038</v>
+      </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="36" t="s">
@@ -18610,7 +18613,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691EC2E3-E9BC-4F88-BC20-9BC4D7BDFAEB}">
   <dimension ref="A1:H169"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>